<commit_message>
computation of different pvalues
</commit_message>
<xml_diff>
--- a/Tables/description_treatment_arms.xlsx
+++ b/Tables/description_treatment_arms.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,13 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D58202C-84C6-48DB-87C1-9CCD650B962F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-645" yWindow="2430" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-645" yWindow="2430" windowWidth="21600" windowHeight="11235"/>
   </bookViews>
   <sheets>
     <sheet name="description_treatment_armss" sheetId="1" r:id="rId1"/>
+    <sheet name="description_treatment_arms" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="46" uniqueCount="27">
   <si>
     <t># cases</t>
   </si>
@@ -131,7 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -163,10 +164,10 @@
       <left/>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color auto="true"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color auto="true"/>
       </bottom>
       <diagonal/>
     </border>
@@ -175,7 +176,7 @@
       <right/>
       <top/>
       <bottom style="double">
-        <color auto="1"/>
+        <color auto="true"/>
       </bottom>
       <diagonal/>
     </border>
@@ -185,26 +186,26 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -224,7 +225,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -375,7 +376,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -399,9 +400,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -425,7 +426,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -460,7 +461,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -478,7 +479,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -503,7 +504,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -519,23 +520,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection sqref="A1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="true"/>
+    <col min="3" max="3" width="18.28515625" customWidth="true"/>
+    <col min="6" max="6" width="26.42578125" customWidth="true"/>
+    <col min="7" max="7" width="21.140625" customWidth="true"/>
+    <col min="8" max="8" width="10" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -559,7 +560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="48">
+    <row r="2" ht="48">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -594,7 +595,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="72">
+    <row r="3" ht="72">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -629,7 +630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="48.75" thickBot="1">
+    <row r="4" ht="48.75" thickBot="true">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -664,8 +665,62 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickTop="1"/>
+    <row r="5" ht="15.75" thickTop="true"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="D2">
+        <v>636</v>
+      </c>
+      <c r="E2">
+        <v>315</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3">
+        <v>1097</v>
+      </c>
+      <c r="E3">
+        <v>768</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4">
+        <v>1922</v>
+      </c>
+      <c r="E4">
+        <v>922</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>